<commit_message>
Added some font style changes
</commit_message>
<xml_diff>
--- a/chit_data.xlsx
+++ b/chit_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rakhil\Documents\Template_chit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD3315E-27E1-4061-A072-4A102086F8CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93426B8F-3012-4B3E-87A4-54A6F597AA7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,20 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -726,7 +713,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -795,6 +782,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -892,7 +885,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -960,6 +953,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1273,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K160"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1292,14 +1287,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
       <c r="G1" s="1"/>
       <c r="H1" s="2"/>
       <c r="I1" s="3"/>
@@ -3030,8 +3025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3046,14 +3041,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="33"/>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
       <c r="I1" s="13"/>
@@ -4736,8 +4731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -4752,14 +4747,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.25" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="33"/>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
       <c r="I1" s="13"/>
@@ -4811,7 +4806,7 @@
         <v>5754</v>
       </c>
       <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:11" ht="19.5" customHeight="1">
       <c r="A4" s="20">
@@ -4833,7 +4828,7 @@
         <v>7332</v>
       </c>
       <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
+      <c r="H4" s="27"/>
     </row>
     <row r="5" spans="1:11" ht="21.75" customHeight="1">
       <c r="A5" s="20">
@@ -4855,7 +4850,7 @@
         <v>4627</v>
       </c>
       <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
+      <c r="H5" s="27"/>
     </row>
     <row r="6" spans="1:11" ht="21.75" customHeight="1">
       <c r="A6" s="20">
@@ -4877,7 +4872,7 @@
         <v>14929</v>
       </c>
       <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
+      <c r="H6" s="27"/>
     </row>
     <row r="7" spans="1:11" ht="21.75" customHeight="1">
       <c r="A7" s="20">
@@ -4899,7 +4894,7 @@
         <v>4588</v>
       </c>
       <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
+      <c r="H7" s="27"/>
     </row>
     <row r="8" spans="1:11" ht="21.75" customHeight="1">
       <c r="A8" s="20">
@@ -4921,7 +4916,7 @@
         <v>5855</v>
       </c>
       <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
+      <c r="H8" s="27"/>
     </row>
     <row r="9" spans="1:11" ht="21.75" customHeight="1">
       <c r="A9" s="20">
@@ -4943,7 +4938,7 @@
         <v>19199</v>
       </c>
       <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
+      <c r="H9" s="27"/>
     </row>
     <row r="10" spans="1:11" ht="21.75" customHeight="1">
       <c r="A10" s="20">
@@ -4953,7 +4948,7 @@
         <v>94</v>
       </c>
       <c r="C10" s="22">
-        <v>0</v>
+        <v>19697</v>
       </c>
       <c r="D10" s="20">
         <v>106</v>
@@ -4965,7 +4960,7 @@
         <v>3575</v>
       </c>
       <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
+      <c r="H10" s="27"/>
     </row>
     <row r="11" spans="1:11" ht="17.25" customHeight="1">
       <c r="A11" s="20">
@@ -4987,7 +4982,7 @@
         <v>4588</v>
       </c>
       <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
+      <c r="H11" s="27"/>
     </row>
     <row r="12" spans="1:11" ht="21.75" customHeight="1">
       <c r="A12" s="20">
@@ -5009,7 +5004,7 @@
         <v>20790</v>
       </c>
       <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
+      <c r="H12" s="27"/>
     </row>
     <row r="13" spans="1:11" ht="18" customHeight="1">
       <c r="A13" s="20">
@@ -5031,7 +5026,7 @@
         <v>10491</v>
       </c>
       <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
+      <c r="H13" s="27"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" customHeight="1">
       <c r="A14" s="20">
@@ -5053,7 +5048,7 @@
         <v>3755</v>
       </c>
       <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
+      <c r="H14" s="27"/>
     </row>
     <row r="15" spans="1:11" ht="17.25" customHeight="1">
       <c r="A15" s="20">
@@ -5075,7 +5070,7 @@
         <v>10554</v>
       </c>
       <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="27"/>
     </row>
     <row r="16" spans="1:11" ht="17.25" customHeight="1">
       <c r="A16" s="20">
@@ -5097,7 +5092,7 @@
         <v>39614</v>
       </c>
       <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
+      <c r="H16" s="27"/>
     </row>
     <row r="17" spans="1:8" ht="18.75" customHeight="1">
       <c r="A17" s="20">
@@ -5119,7 +5114,7 @@
         <v>3266</v>
       </c>
       <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
+      <c r="H17" s="27"/>
     </row>
     <row r="18" spans="1:8" ht="17.25" customHeight="1">
       <c r="A18" s="20">
@@ -5141,7 +5136,7 @@
         <v>8925</v>
       </c>
       <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
+      <c r="H18" s="27"/>
     </row>
     <row r="19" spans="1:8" ht="21.75" customHeight="1">
       <c r="A19" s="20">
@@ -5163,7 +5158,7 @@
         <v>20661</v>
       </c>
       <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
+      <c r="H19" s="27"/>
     </row>
     <row r="20" spans="1:8" ht="21.75" customHeight="1">
       <c r="A20" s="20">
@@ -5185,7 +5180,7 @@
         <v>15208</v>
       </c>
       <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
+      <c r="H20" s="27"/>
     </row>
     <row r="21" spans="1:8" ht="21.75" customHeight="1">
       <c r="A21" s="20">
@@ -5207,7 +5202,7 @@
         <v>9370</v>
       </c>
       <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
+      <c r="H21" s="27"/>
     </row>
     <row r="22" spans="1:8" ht="18" customHeight="1">
       <c r="A22" s="20">
@@ -5229,7 +5224,7 @@
         <v>28347</v>
       </c>
       <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
+      <c r="H22" s="27"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1">
       <c r="A23" s="20">
@@ -5251,7 +5246,7 @@
         <v>24403</v>
       </c>
       <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
+      <c r="H23" s="27"/>
     </row>
     <row r="24" spans="1:8" ht="18" customHeight="1">
       <c r="A24" s="20">
@@ -5273,7 +5268,7 @@
         <v>9177</v>
       </c>
       <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
+      <c r="H24" s="27"/>
     </row>
     <row r="25" spans="1:8" ht="21.75" customHeight="1">
       <c r="A25" s="20">
@@ -5295,7 +5290,7 @@
         <v>11599</v>
       </c>
       <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
+      <c r="H25" s="27"/>
     </row>
     <row r="26" spans="1:8" ht="21.75" customHeight="1">
       <c r="A26" s="20">
@@ -5317,7 +5312,7 @@
         <v>14421</v>
       </c>
       <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
+      <c r="H26" s="27"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" customHeight="1">
       <c r="A27" s="20">
@@ -5339,7 +5334,7 @@
         <v>24430</v>
       </c>
       <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
+      <c r="H27" s="27"/>
     </row>
     <row r="28" spans="1:8" ht="21.75" customHeight="1">
       <c r="A28" s="20">
@@ -5361,7 +5356,7 @@
         <v>9865</v>
       </c>
       <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
+      <c r="H28" s="27"/>
     </row>
     <row r="29" spans="1:8" ht="19.5" customHeight="1">
       <c r="A29" s="20">
@@ -5383,7 +5378,7 @@
         <v>12691</v>
       </c>
       <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
+      <c r="H29" s="27"/>
     </row>
     <row r="30" spans="1:8" ht="21.75" customHeight="1">
       <c r="A30" s="20">
@@ -5405,7 +5400,7 @@
         <v>31522</v>
       </c>
       <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
+      <c r="H30" s="27"/>
     </row>
     <row r="31" spans="1:8" ht="18" customHeight="1">
       <c r="A31" s="20">
@@ -5427,7 +5422,7 @@
         <v>44445</v>
       </c>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="27"/>
     </row>
     <row r="32" spans="1:8" ht="28.5" customHeight="1">
       <c r="A32" s="20">
@@ -5437,7 +5432,7 @@
         <v>138</v>
       </c>
       <c r="C32" s="22">
-        <v>63074</v>
+        <v>102382</v>
       </c>
       <c r="D32" s="20">
         <v>128</v>
@@ -5445,7 +5440,7 @@
       <c r="E32" s="18"/>
       <c r="F32" s="23"/>
       <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
+      <c r="H32" s="27"/>
     </row>
     <row r="33" spans="1:8" ht="16.5" customHeight="1">
       <c r="A33" s="20">
@@ -5463,7 +5458,7 @@
       <c r="E33" s="18"/>
       <c r="F33" s="23"/>
       <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
+      <c r="H33" s="27"/>
     </row>
     <row r="34" spans="1:8" ht="21.75" customHeight="1">
       <c r="A34" s="20">
@@ -5481,7 +5476,7 @@
       <c r="E34" s="13"/>
       <c r="F34" s="23"/>
       <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
+      <c r="H34" s="27"/>
     </row>
     <row r="35" spans="1:8" ht="17.25" customHeight="1">
       <c r="A35" s="20">
@@ -5499,7 +5494,7 @@
       <c r="E35" s="18"/>
       <c r="F35" s="23"/>
       <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
+      <c r="H35" s="27"/>
     </row>
     <row r="36" spans="1:8" ht="18.75" customHeight="1">
       <c r="A36" s="7">
@@ -5517,7 +5512,7 @@
       <c r="E36" s="18"/>
       <c r="F36" s="22"/>
       <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
+      <c r="H36" s="27"/>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1">
       <c r="A37" s="20">
@@ -5534,6 +5529,7 @@
       </c>
       <c r="E37" s="18"/>
       <c r="F37" s="22"/>
+      <c r="H37" s="27"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1">
       <c r="A38" s="20">
@@ -5550,6 +5546,7 @@
       </c>
       <c r="E38" s="18"/>
       <c r="F38" s="23"/>
+      <c r="H38" s="27"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1">
       <c r="A39" s="7">
@@ -5566,6 +5563,7 @@
       </c>
       <c r="E39" s="18"/>
       <c r="F39" s="22"/>
+      <c r="H39" s="27"/>
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1">
       <c r="A40" s="20">
@@ -5582,12 +5580,13 @@
       </c>
       <c r="E40" s="18"/>
       <c r="F40" s="22"/>
+      <c r="H40" s="27"/>
     </row>
     <row r="41" spans="1:8" ht="15.75" customHeight="1">
       <c r="A41" s="12"/>
       <c r="B41" s="13"/>
       <c r="C41">
-        <v>542621</v>
+        <v>601626</v>
       </c>
       <c r="D41" s="12"/>
       <c r="E41" s="13"/>
@@ -5608,8 +5607,8 @@
       <c r="E43" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="F43">
-        <v>2311025</v>
+      <c r="F43" s="28">
+        <v>2370030</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1">

</xml_diff>